<commit_message>
Corrected calculation in BNVFE
</commit_message>
<xml_diff>
--- a/InputData/trans/BNVFE/BAU New Veh Fuel Economy.xlsx
+++ b/InputData/trans/BNVFE/BAU New Veh Fuel Economy.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\Brazil\Model\InputData\trans\BNVFE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\trans\BNVFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3D447C-C86A-4BE5-8409-D54692E1F7A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" firstSheet="21" activeTab="22" xr2:uid="{730F6D5A-6C3B-47E7-AA94-50A9B9E008D1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19395" windowHeight="10395" firstSheet="18" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -71,7 +70,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1258,7 +1257,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="12">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -2557,176 +2556,176 @@
     <xf numFmtId="9" fontId="0" fillId="40" borderId="0" xfId="153" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="34" borderId="0" xfId="153" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="40" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="40" borderId="26" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="40" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="40" borderId="26" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="156">
-    <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Body: normal cell 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Calculation 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Check Cell 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Column heading" xfId="36" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="8"/>
+    <cellStyle name="20% - Accent2 2" xfId="9"/>
+    <cellStyle name="20% - Accent3 2" xfId="10"/>
+    <cellStyle name="20% - Accent4 2" xfId="11"/>
+    <cellStyle name="20% - Accent5 2" xfId="12"/>
+    <cellStyle name="20% - Accent6 2" xfId="13"/>
+    <cellStyle name="40% - Accent1 2" xfId="14"/>
+    <cellStyle name="40% - Accent2 2" xfId="15"/>
+    <cellStyle name="40% - Accent3 2" xfId="16"/>
+    <cellStyle name="40% - Accent4 2" xfId="17"/>
+    <cellStyle name="40% - Accent5 2" xfId="18"/>
+    <cellStyle name="40% - Accent6 2" xfId="19"/>
+    <cellStyle name="60% - Accent1 2" xfId="20"/>
+    <cellStyle name="60% - Accent2 2" xfId="21"/>
+    <cellStyle name="60% - Accent3 2" xfId="22"/>
+    <cellStyle name="60% - Accent4 2" xfId="23"/>
+    <cellStyle name="60% - Accent5 2" xfId="24"/>
+    <cellStyle name="60% - Accent6 2" xfId="25"/>
+    <cellStyle name="Accent1 2" xfId="26"/>
+    <cellStyle name="Accent2 2" xfId="27"/>
+    <cellStyle name="Accent3 2" xfId="28"/>
+    <cellStyle name="Accent4 2" xfId="29"/>
+    <cellStyle name="Accent5 2" xfId="30"/>
+    <cellStyle name="Accent6 2" xfId="31"/>
+    <cellStyle name="Bad 2" xfId="32"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Body: normal cell 2" xfId="33"/>
+    <cellStyle name="Calculation 2" xfId="34"/>
+    <cellStyle name="Check Cell 2" xfId="35"/>
+    <cellStyle name="Column heading" xfId="36"/>
     <cellStyle name="Comma" xfId="155" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="37" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Comma 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Comma 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Comma 4" xfId="40" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Comma 5" xfId="41" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Comma 6" xfId="42" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Comma 7" xfId="43" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Comma 8" xfId="44" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Corner heading" xfId="45" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Currency 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Currency 3" xfId="47" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Currency 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Data" xfId="49" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Data 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Data no deci" xfId="51" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Data Superscript" xfId="52" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="53" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Footnotes: top row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Good 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Header: bottom row 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Heading 1 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Heading 2 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Heading 3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Heading 4 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Hed Side" xfId="63" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Hed Side 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Hed Side bold" xfId="65" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Hed Side Indent" xfId="66" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="68" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Hed Top" xfId="69" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Hed Top - SECTION" xfId="70" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Hed Top_3-new4" xfId="71" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Comma 2" xfId="37"/>
+    <cellStyle name="Comma 2 2" xfId="38"/>
+    <cellStyle name="Comma 3" xfId="39"/>
+    <cellStyle name="Comma 4" xfId="40"/>
+    <cellStyle name="Comma 5" xfId="41"/>
+    <cellStyle name="Comma 6" xfId="42"/>
+    <cellStyle name="Comma 7" xfId="43"/>
+    <cellStyle name="Comma 8" xfId="44"/>
+    <cellStyle name="Corner heading" xfId="45"/>
+    <cellStyle name="Currency 2" xfId="46"/>
+    <cellStyle name="Currency 3" xfId="47"/>
+    <cellStyle name="Currency 3 2" xfId="48"/>
+    <cellStyle name="Data" xfId="49"/>
+    <cellStyle name="Data 2" xfId="50"/>
+    <cellStyle name="Data no deci" xfId="51"/>
+    <cellStyle name="Data Superscript" xfId="52"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="53"/>
+    <cellStyle name="Explanatory Text 2" xfId="54"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55"/>
+    <cellStyle name="Footnotes: top row" xfId="2"/>
+    <cellStyle name="Footnotes: top row 2" xfId="56"/>
+    <cellStyle name="Good 2" xfId="57"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
+    <cellStyle name="Header: bottom row 2" xfId="58"/>
+    <cellStyle name="Heading 1 2" xfId="59"/>
+    <cellStyle name="Heading 2 2" xfId="60"/>
+    <cellStyle name="Heading 3 2" xfId="61"/>
+    <cellStyle name="Heading 4 2" xfId="62"/>
+    <cellStyle name="Hed Side" xfId="63"/>
+    <cellStyle name="Hed Side 2" xfId="64"/>
+    <cellStyle name="Hed Side bold" xfId="65"/>
+    <cellStyle name="Hed Side Indent" xfId="66"/>
+    <cellStyle name="Hed Side Regular" xfId="67"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="68"/>
+    <cellStyle name="Hed Top" xfId="69"/>
+    <cellStyle name="Hed Top - SECTION" xfId="70"/>
+    <cellStyle name="Hed Top_3-new4" xfId="71"/>
     <cellStyle name="Hyperlink" xfId="154" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Input 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Neutral 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="72"/>
+    <cellStyle name="Input 2" xfId="73"/>
+    <cellStyle name="Linked Cell 2" xfId="74"/>
+    <cellStyle name="Neutral 2" xfId="75"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="76" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 11" xfId="77" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 3 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="84" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 3 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="88" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 3 4" xfId="89" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="90" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 3 5" xfId="91" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 3 6" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 3 7" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 4" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 4 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 4 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 4 2 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 4 3" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 4 3 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 4 3 3" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 4 4" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 4 4 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 4 5" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 4 6" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 4 7" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 5" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 5 2" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 5 3" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 6 2" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 7" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 7 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 8" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 9" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Note 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Note 2 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Output 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Parent row 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Normal 10" xfId="76"/>
+    <cellStyle name="Normal 11" xfId="77"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="78"/>
+    <cellStyle name="Normal 2 3" xfId="79"/>
+    <cellStyle name="Normal 3" xfId="80"/>
+    <cellStyle name="Normal 3 2" xfId="81"/>
+    <cellStyle name="Normal 3 2 2" xfId="82"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="83"/>
+    <cellStyle name="Normal 3 2 3" xfId="84"/>
+    <cellStyle name="Normal 3 3" xfId="85"/>
+    <cellStyle name="Normal 3 3 2" xfId="86"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="87"/>
+    <cellStyle name="Normal 3 3 3" xfId="88"/>
+    <cellStyle name="Normal 3 4" xfId="89"/>
+    <cellStyle name="Normal 3 4 2" xfId="90"/>
+    <cellStyle name="Normal 3 5" xfId="91"/>
+    <cellStyle name="Normal 3 6" xfId="92"/>
+    <cellStyle name="Normal 3 7" xfId="93"/>
+    <cellStyle name="Normal 4" xfId="94"/>
+    <cellStyle name="Normal 4 2" xfId="95"/>
+    <cellStyle name="Normal 4 2 2" xfId="96"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="97"/>
+    <cellStyle name="Normal 4 2 3" xfId="98"/>
+    <cellStyle name="Normal 4 3" xfId="99"/>
+    <cellStyle name="Normal 4 3 2" xfId="100"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="101"/>
+    <cellStyle name="Normal 4 3 3" xfId="102"/>
+    <cellStyle name="Normal 4 4" xfId="103"/>
+    <cellStyle name="Normal 4 4 2" xfId="104"/>
+    <cellStyle name="Normal 4 5" xfId="105"/>
+    <cellStyle name="Normal 4 6" xfId="106"/>
+    <cellStyle name="Normal 4 7" xfId="107"/>
+    <cellStyle name="Normal 5" xfId="108"/>
+    <cellStyle name="Normal 5 2" xfId="109"/>
+    <cellStyle name="Normal 5 3" xfId="110"/>
+    <cellStyle name="Normal 6" xfId="111"/>
+    <cellStyle name="Normal 6 2" xfId="112"/>
+    <cellStyle name="Normal 7" xfId="113"/>
+    <cellStyle name="Normal 7 2" xfId="114"/>
+    <cellStyle name="Normal 8" xfId="115"/>
+    <cellStyle name="Normal 9" xfId="116"/>
+    <cellStyle name="Note 2" xfId="117"/>
+    <cellStyle name="Note 2 2" xfId="118"/>
+    <cellStyle name="Output 2" xfId="119"/>
+    <cellStyle name="Parent row" xfId="3"/>
+    <cellStyle name="Parent row 2" xfId="120"/>
     <cellStyle name="Percent" xfId="153" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Percent 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Percent 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Percent 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Percent 4" xfId="125" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Reference" xfId="126" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Row heading" xfId="127" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Source Hed" xfId="128" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Source Letter" xfId="129" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Source Superscript" xfId="130" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Source Superscript 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Source Text" xfId="132" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Source Text 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="State" xfId="134" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Superscript" xfId="135" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Table Data" xfId="136" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Table Head Top" xfId="137" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Table Hed Side" xfId="138" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Table title 2" xfId="139" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Title Text" xfId="141" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Title Text 1" xfId="142" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Title Text 2" xfId="143" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Title-1" xfId="144" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Title-2" xfId="145" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Title-3" xfId="146" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Total 2" xfId="147" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Warning Text 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Wrap" xfId="149" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Wrap Bold" xfId="150" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Wrap Title" xfId="151" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="152" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Percent 2" xfId="121"/>
+    <cellStyle name="Percent 2 2" xfId="122"/>
+    <cellStyle name="Percent 3" xfId="123"/>
+    <cellStyle name="Percent 3 2" xfId="124"/>
+    <cellStyle name="Percent 4" xfId="125"/>
+    <cellStyle name="Reference" xfId="126"/>
+    <cellStyle name="Row heading" xfId="127"/>
+    <cellStyle name="Source Hed" xfId="128"/>
+    <cellStyle name="Source Letter" xfId="129"/>
+    <cellStyle name="Source Superscript" xfId="130"/>
+    <cellStyle name="Source Superscript 2" xfId="131"/>
+    <cellStyle name="Source Text" xfId="132"/>
+    <cellStyle name="Source Text 2" xfId="133"/>
+    <cellStyle name="State" xfId="134"/>
+    <cellStyle name="Superscript" xfId="135"/>
+    <cellStyle name="Table Data" xfId="136"/>
+    <cellStyle name="Table Head Top" xfId="137"/>
+    <cellStyle name="Table Hed Side" xfId="138"/>
+    <cellStyle name="Table title" xfId="7"/>
+    <cellStyle name="Table title 2" xfId="139"/>
+    <cellStyle name="Title 2" xfId="140"/>
+    <cellStyle name="Title Text" xfId="141"/>
+    <cellStyle name="Title Text 1" xfId="142"/>
+    <cellStyle name="Title Text 2" xfId="143"/>
+    <cellStyle name="Title-1" xfId="144"/>
+    <cellStyle name="Title-2" xfId="145"/>
+    <cellStyle name="Title-3" xfId="146"/>
+    <cellStyle name="Total 2" xfId="147"/>
+    <cellStyle name="Warning Text 2" xfId="148"/>
+    <cellStyle name="Wrap" xfId="149"/>
+    <cellStyle name="Wrap Bold" xfId="150"/>
+    <cellStyle name="Wrap Title" xfId="151"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="152"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3542,23 +3541,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3594,23 +3576,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3786,7 +3751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD190"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37341,15 +37306,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B63" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B26" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B34" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B56" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B41" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B78" r:id="rId9" xr:uid="{88250872-3BE8-4809-AAF6-4E90E919070B}"/>
+    <hyperlink ref="B63" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B17" r:id="rId3"/>
+    <hyperlink ref="B26" r:id="rId4"/>
+    <hyperlink ref="B34" r:id="rId5"/>
+    <hyperlink ref="B48" r:id="rId6"/>
+    <hyperlink ref="B56" r:id="rId7"/>
+    <hyperlink ref="B41" r:id="rId8"/>
+    <hyperlink ref="B78" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -37357,7 +37322,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37561,7 +37526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37611,7 +37576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37641,7 +37606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37690,7 +37655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37805,7 +37770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37907,7 +37872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38069,7 +38034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38215,7 +38180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38289,7 +38254,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38387,40 +38352,40 @@
       <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:14" ht="21">
-      <c r="A14" s="105" t="s">
+      <c r="A14" s="111" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="105"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="105"/>
-      <c r="N14" s="105"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="111"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
+      <c r="K14" s="111"/>
+      <c r="L14" s="111"/>
+      <c r="M14" s="111"/>
+      <c r="N14" s="111"/>
     </row>
     <row r="15" spans="1:14" ht="16.149999999999999" thickBot="1">
-      <c r="A15" s="106" t="s">
+      <c r="A15" s="112" t="s">
         <v>243</v>
       </c>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="106"/>
-      <c r="M15" s="106"/>
-      <c r="N15" s="106"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="112"/>
     </row>
     <row r="16" spans="1:14" ht="14.65" thickBot="1">
       <c r="A16" s="43"/>
@@ -40796,14 +40761,14 @@
     <mergeCell ref="A15:N15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1" xr:uid="{90B25065-98AF-40EC-9EC5-C549B8D2D7C0}"/>
+    <hyperlink ref="I8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -40959,8 +40924,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D18" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D19" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D18" r:id="rId1"/>
+    <hyperlink ref="D19" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -40968,7 +40933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -41023,7 +40988,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -41031,7 +40996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780079A6-729A-4BF6-A60D-8613DB4EC2FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -41044,7 +41009,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41125,11 +41090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -41688,7 +41653,7 @@
       <c r="F11">
         <v>8.7048677754535786E-2</v>
       </c>
-      <c r="I11" s="107" t="s">
+      <c r="I11" s="105" t="s">
         <v>384</v>
       </c>
     </row>
@@ -42182,139 +42147,139 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="K16" s="108">
+      <c r="K16" s="106">
         <f>SUM(K13:K15)</f>
         <v>120062285703208.23</v>
       </c>
-      <c r="L16" s="108">
+      <c r="L16" s="106">
         <f t="shared" ref="L16:AR16" si="0">SUM(L13:L15)</f>
         <v>125222436550851.09</v>
       </c>
-      <c r="M16" s="108">
+      <c r="M16" s="106">
         <f t="shared" si="0"/>
         <v>130841787410825.59</v>
       </c>
-      <c r="N16" s="108">
+      <c r="N16" s="106">
         <f t="shared" si="0"/>
         <v>136954936909647.2</v>
       </c>
-      <c r="O16" s="108">
+      <c r="O16" s="106">
         <f t="shared" si="0"/>
         <v>143651317601530.53</v>
       </c>
-      <c r="P16" s="108">
+      <c r="P16" s="106">
         <f t="shared" si="0"/>
         <v>150985989668157</v>
       </c>
-      <c r="Q16" s="108">
+      <c r="Q16" s="106">
         <f t="shared" si="0"/>
         <v>158980245644967.91</v>
       </c>
-      <c r="R16" s="108">
+      <c r="R16" s="106">
         <f t="shared" si="0"/>
         <v>167612909015385.47</v>
       </c>
-      <c r="S16" s="108">
+      <c r="S16" s="106">
         <f t="shared" si="0"/>
         <v>176226946308777.75</v>
       </c>
-      <c r="T16" s="108">
+      <c r="T16" s="106">
         <f t="shared" si="0"/>
         <v>184273479514302.25</v>
       </c>
-      <c r="U16" s="108">
+      <c r="U16" s="106">
         <f t="shared" si="0"/>
         <v>191799878334263.22</v>
       </c>
-      <c r="V16" s="108">
+      <c r="V16" s="106">
         <f t="shared" si="0"/>
         <v>198838374046822.38</v>
       </c>
-      <c r="W16" s="108">
+      <c r="W16" s="106">
         <f t="shared" si="0"/>
         <v>205419107525463</v>
       </c>
-      <c r="X16" s="108">
+      <c r="X16" s="106">
         <f t="shared" si="0"/>
         <v>211570277896100</v>
       </c>
-      <c r="Y16" s="108">
+      <c r="Y16" s="106">
         <f t="shared" si="0"/>
         <v>217336000393173.84</v>
       </c>
-      <c r="Z16" s="108">
+      <c r="Z16" s="106">
         <f t="shared" si="0"/>
         <v>222755892217345.38</v>
       </c>
-      <c r="AA16" s="108">
+      <c r="AA16" s="106">
         <f t="shared" si="0"/>
         <v>227862150680357.19</v>
       </c>
-      <c r="AB16" s="108">
+      <c r="AB16" s="106">
         <f t="shared" si="0"/>
         <v>232691363772114.59</v>
       </c>
-      <c r="AC16" s="108">
+      <c r="AC16" s="106">
         <f t="shared" si="0"/>
         <v>237102223499737.22</v>
       </c>
-      <c r="AD16" s="108">
+      <c r="AD16" s="106">
         <f t="shared" si="0"/>
         <v>241017198099816.56</v>
       </c>
-      <c r="AE16" s="108">
+      <c r="AE16" s="106">
         <f t="shared" si="0"/>
         <v>244497221223826.41</v>
       </c>
-      <c r="AF16" s="108">
+      <c r="AF16" s="106">
         <f t="shared" si="0"/>
         <v>247574100504740.09</v>
       </c>
-      <c r="AG16" s="108">
+      <c r="AG16" s="106">
         <f t="shared" si="0"/>
         <v>250293751878965</v>
       </c>
-      <c r="AH16" s="108">
+      <c r="AH16" s="106">
         <f t="shared" si="0"/>
         <v>252696972462987.28</v>
       </c>
-      <c r="AI16" s="108">
+      <c r="AI16" s="106">
         <f t="shared" si="0"/>
         <v>254822131381383.34</v>
       </c>
-      <c r="AJ16" s="108">
+      <c r="AJ16" s="106">
         <f t="shared" si="0"/>
         <v>256704382678802.69</v>
       </c>
-      <c r="AK16" s="108">
+      <c r="AK16" s="106">
         <f t="shared" si="0"/>
         <v>258374696279324.5</v>
       </c>
-      <c r="AL16" s="108">
+      <c r="AL16" s="106">
         <f t="shared" si="0"/>
         <v>259862086903347.5</v>
       </c>
-      <c r="AM16" s="108">
+      <c r="AM16" s="106">
         <f t="shared" si="0"/>
         <v>261191839526366.16</v>
       </c>
-      <c r="AN16" s="108">
+      <c r="AN16" s="106">
         <f t="shared" si="0"/>
         <v>262388277951264.31</v>
       </c>
-      <c r="AO16" s="108">
+      <c r="AO16" s="106">
         <f t="shared" si="0"/>
         <v>263473146983350.19</v>
       </c>
-      <c r="AP16" s="108">
+      <c r="AP16" s="106">
         <f t="shared" si="0"/>
         <v>264464945107297.25</v>
       </c>
-      <c r="AQ16" s="108">
+      <c r="AQ16" s="106">
         <f t="shared" si="0"/>
         <v>265379784616347.31</v>
       </c>
-      <c r="AR16" s="108">
+      <c r="AR16" s="106">
         <f t="shared" si="0"/>
         <v>266231285184595.69</v>
       </c>
@@ -42436,139 +42401,139 @@
       <c r="I19" t="s">
         <v>387</v>
       </c>
-      <c r="K19" s="111">
+      <c r="K19" s="109">
         <f>K18*10^3</f>
         <v>164878851200</v>
       </c>
-      <c r="L19" s="111">
+      <c r="L19" s="109">
         <f t="shared" ref="L19:AR19" si="1">L18*10^3</f>
         <v>172476613600.00003</v>
       </c>
-      <c r="M19" s="111">
+      <c r="M19" s="109">
         <f t="shared" si="1"/>
         <v>180682556000</v>
       </c>
-      <c r="N19" s="111">
+      <c r="N19" s="109">
         <f t="shared" si="1"/>
         <v>189542353200</v>
       </c>
-      <c r="O19" s="111">
+      <c r="O19" s="109">
         <f t="shared" si="1"/>
         <v>199181827200</v>
       </c>
-      <c r="P19" s="111">
+      <c r="P19" s="109">
         <f t="shared" si="1"/>
         <v>209680173600.00003</v>
       </c>
-      <c r="Q19" s="111">
+      <c r="Q19" s="109">
         <f t="shared" si="1"/>
         <v>221066006399.99997</v>
       </c>
-      <c r="R19" s="111">
+      <c r="R19" s="109">
         <f t="shared" si="1"/>
         <v>233314040400</v>
       </c>
-      <c r="S19" s="111">
+      <c r="S19" s="109">
         <f t="shared" si="1"/>
         <v>245509882400</v>
       </c>
-      <c r="T19" s="111">
+      <c r="T19" s="109">
         <f t="shared" si="1"/>
         <v>256889526400</v>
       </c>
-      <c r="U19" s="111">
+      <c r="U19" s="109">
         <f t="shared" si="1"/>
         <v>267522012400</v>
       </c>
-      <c r="V19" s="111">
+      <c r="V19" s="109">
         <f t="shared" si="1"/>
         <v>277454900800</v>
       </c>
-      <c r="W19" s="111">
+      <c r="W19" s="109">
         <f t="shared" si="1"/>
         <v>286732554800</v>
       </c>
-      <c r="X19" s="111">
+      <c r="X19" s="109">
         <f t="shared" si="1"/>
         <v>295396411600</v>
       </c>
-      <c r="Y19" s="111">
+      <c r="Y19" s="109">
         <f t="shared" si="1"/>
         <v>303509750000</v>
       </c>
-      <c r="Z19" s="111">
+      <c r="Z19" s="109">
         <f t="shared" si="1"/>
         <v>311128921200</v>
       </c>
-      <c r="AA19" s="111">
+      <c r="AA19" s="109">
         <f t="shared" si="1"/>
         <v>318299719200</v>
       </c>
-      <c r="AB19" s="111">
+      <c r="AB19" s="109">
         <f t="shared" si="1"/>
         <v>325074235200</v>
       </c>
-      <c r="AC19" s="111">
+      <c r="AC19" s="109">
         <f t="shared" si="1"/>
         <v>331258311600</v>
       </c>
-      <c r="AD19" s="111">
+      <c r="AD19" s="109">
         <f t="shared" si="1"/>
         <v>336744190000</v>
       </c>
-      <c r="AE19" s="111">
+      <c r="AE19" s="109">
         <f t="shared" si="1"/>
         <v>341618388800</v>
       </c>
-      <c r="AF19" s="111">
+      <c r="AF19" s="109">
         <f t="shared" si="1"/>
         <v>345928121200</v>
       </c>
-      <c r="AG19" s="111">
+      <c r="AG19" s="109">
         <f t="shared" si="1"/>
         <v>349737644800</v>
       </c>
-      <c r="AH19" s="111">
+      <c r="AH19" s="109">
         <f t="shared" si="1"/>
         <v>353104055600</v>
       </c>
-      <c r="AI19" s="111">
+      <c r="AI19" s="109">
         <f t="shared" si="1"/>
         <v>356081074400</v>
       </c>
-      <c r="AJ19" s="111">
+      <c r="AJ19" s="109">
         <f t="shared" si="1"/>
         <v>358717915600</v>
       </c>
-      <c r="AK19" s="111">
+      <c r="AK19" s="109">
         <f t="shared" si="1"/>
         <v>361057940400</v>
       </c>
-      <c r="AL19" s="111">
+      <c r="AL19" s="109">
         <f t="shared" si="1"/>
         <v>363141744800</v>
       </c>
-      <c r="AM19" s="111">
+      <c r="AM19" s="109">
         <f t="shared" si="1"/>
         <v>365004732400</v>
       </c>
-      <c r="AN19" s="111">
+      <c r="AN19" s="109">
         <f t="shared" si="1"/>
         <v>366680940000</v>
       </c>
-      <c r="AO19" s="111">
+      <c r="AO19" s="109">
         <f t="shared" si="1"/>
         <v>368200799200.00006</v>
       </c>
-      <c r="AP19" s="111">
+      <c r="AP19" s="109">
         <f t="shared" si="1"/>
         <v>369590208400</v>
       </c>
-      <c r="AQ19" s="111">
+      <c r="AQ19" s="109">
         <f t="shared" si="1"/>
         <v>370871730400</v>
       </c>
-      <c r="AR19" s="111">
+      <c r="AR19" s="109">
         <f t="shared" si="1"/>
         <v>372064458400</v>
       </c>
@@ -42577,139 +42542,139 @@
       <c r="I20" t="s">
         <v>385</v>
       </c>
-      <c r="K20" s="110">
+      <c r="K20" s="108">
         <f>K19*units_convertor!$A$2</f>
         <v>102450936648.99519</v>
       </c>
-      <c r="L20" s="110">
+      <c r="L20" s="108">
         <f>L19*units_convertor!$A$2</f>
         <v>107171965869.24562</v>
       </c>
-      <c r="M20" s="110">
+      <c r="M20" s="108">
         <f>M19*units_convertor!$A$2</f>
         <v>112270900504.276</v>
       </c>
-      <c r="N20" s="110">
+      <c r="N20" s="108">
         <f>N19*units_convertor!$A$2</f>
         <v>117776121550.2372</v>
       </c>
-      <c r="O20" s="110">
+      <c r="O20" s="108">
         <f>O19*units_convertor!$A$2</f>
         <v>123765811149.0912</v>
       </c>
-      <c r="P20" s="110">
+      <c r="P20" s="108">
         <f>P19*units_convertor!$A$2</f>
         <v>130289179150.00562</v>
       </c>
-      <c r="Q20" s="110">
+      <c r="Q20" s="108">
         <f>Q19*units_convertor!$A$2</f>
         <v>137364005462.77438</v>
       </c>
-      <c r="R20" s="110">
+      <c r="R20" s="108">
         <f>R19*units_convertor!$A$2</f>
         <v>144974578597.3884</v>
       </c>
-      <c r="S20" s="110">
+      <c r="S20" s="108">
         <f>S19*units_convertor!$A$2</f>
         <v>152552721136.77042</v>
       </c>
-      <c r="T20" s="110">
+      <c r="T20" s="108">
         <f>T19*units_convertor!$A$2</f>
         <v>159623701908.6944</v>
       </c>
-      <c r="U20" s="110">
+      <c r="U20" s="108">
         <f>U19*units_convertor!$A$2</f>
         <v>166230420367.0004</v>
       </c>
-      <c r="V20" s="110">
+      <c r="V20" s="108">
         <f>V19*units_convertor!$A$2</f>
         <v>172402429164.9968</v>
       </c>
-      <c r="W20" s="110">
+      <c r="W20" s="108">
         <f>W19*units_convertor!$A$2</f>
         <v>178167294308.6308</v>
       </c>
-      <c r="X20" s="110">
+      <c r="X20" s="108">
         <f>X19*units_convertor!$A$2</f>
         <v>183550763672.30359</v>
       </c>
-      <c r="Y20" s="110">
+      <c r="Y20" s="108">
         <f>Y19*units_convertor!$A$2</f>
         <v>188592156867.25</v>
       </c>
-      <c r="Z20" s="110">
+      <c r="Z20" s="108">
         <f>Z19*units_convertor!$A$2</f>
         <v>193326488894.96521</v>
       </c>
-      <c r="AA20" s="110">
+      <c r="AA20" s="108">
         <f>AA19*units_convertor!$A$2</f>
         <v>197782214819.02319</v>
       </c>
-      <c r="AB20" s="110">
+      <c r="AB20" s="108">
         <f>AB19*units_convertor!$A$2</f>
         <v>201991702600.4592</v>
       </c>
-      <c r="AC20" s="110">
+      <c r="AC20" s="108">
         <f>AC19*units_convertor!$A$2</f>
         <v>205834308337.20361</v>
       </c>
-      <c r="AD20" s="110">
+      <c r="AD20" s="108">
         <f>AD19*units_convertor!$A$2</f>
         <v>209243074084.48999</v>
       </c>
-      <c r="AE20" s="110">
+      <c r="AE20" s="108">
         <f>AE19*units_convertor!$A$2</f>
         <v>212271759867.0448</v>
       </c>
-      <c r="AF20" s="110">
+      <c r="AF20" s="108">
         <f>AF19*units_convertor!$A$2</f>
         <v>214949702598.16519</v>
       </c>
-      <c r="AG20" s="110">
+      <c r="AG20" s="108">
         <f>AG19*units_convertor!$A$2</f>
         <v>217316830087.02081</v>
       </c>
-      <c r="AH20" s="110">
+      <c r="AH20" s="108">
         <f>AH19*units_convertor!$A$2</f>
         <v>219408620132.2276</v>
       </c>
-      <c r="AI20" s="110">
+      <c r="AI20" s="108">
         <f>AI19*units_convertor!$A$2</f>
         <v>221258453281.00241</v>
       </c>
-      <c r="AJ20" s="110">
+      <c r="AJ20" s="108">
         <f>AJ19*units_convertor!$A$2</f>
         <v>222896909934.2876</v>
       </c>
-      <c r="AK20" s="110">
+      <c r="AK20" s="108">
         <f>AK19*units_convertor!$A$2</f>
         <v>224350933484.28839</v>
       </c>
-      <c r="AL20" s="110">
+      <c r="AL20" s="108">
         <f>AL19*units_convertor!$A$2</f>
         <v>225645749108.12079</v>
       </c>
-      <c r="AM20" s="110">
+      <c r="AM20" s="108">
         <f>AM19*units_convertor!$A$2</f>
         <v>226803355576.12039</v>
       </c>
-      <c r="AN20" s="110">
+      <c r="AN20" s="108">
         <f>AN19*units_convertor!$A$2</f>
         <v>227844902368.73999</v>
       </c>
-      <c r="AO20" s="110">
+      <c r="AO20" s="108">
         <f>AO19*units_convertor!$A$2</f>
         <v>228789298799.70325</v>
       </c>
-      <c r="AP20" s="110">
+      <c r="AP20" s="108">
         <f>AP19*units_convertor!$A$2</f>
         <v>229652637383.7164</v>
       </c>
-      <c r="AQ20" s="110">
+      <c r="AQ20" s="108">
         <f>AQ19*units_convertor!$A$2</f>
         <v>230448937990.37839</v>
       </c>
-      <c r="AR20" s="110">
+      <c r="AR20" s="108">
         <f>AR19*units_convertor!$A$2</f>
         <v>231190064580.4664</v>
       </c>
@@ -42857,139 +42822,139 @@
       <c r="I22" t="s">
         <v>386</v>
       </c>
-      <c r="K22" s="112">
+      <c r="K22" s="110">
         <f>K20/K16</f>
         <v>8.5331489442281672E-4</v>
       </c>
-      <c r="L22" s="109">
+      <c r="L22" s="107">
         <f t="shared" ref="L22:AR22" si="3">L20/L16</f>
         <v>8.5585274349556822E-4</v>
       </c>
-      <c r="M22" s="109">
+      <c r="M22" s="107">
         <f t="shared" si="3"/>
         <v>8.5806608672931448E-4</v>
       </c>
-      <c r="N22" s="109">
+      <c r="N22" s="107">
         <f t="shared" si="3"/>
         <v>8.5996258483136848E-4</v>
       </c>
-      <c r="O22" s="109">
+      <c r="O22" s="107">
         <f t="shared" si="3"/>
         <v>8.6157101247341802E-4</v>
       </c>
-      <c r="P22" s="109">
+      <c r="P22" s="107">
         <f t="shared" si="3"/>
         <v>8.62922311112179E-4</v>
       </c>
-      <c r="Q22" s="109">
+      <c r="Q22" s="107">
         <f t="shared" si="3"/>
         <v>8.6403191104342258E-4</v>
       </c>
-      <c r="R22" s="109">
+      <c r="R22" s="107">
         <f t="shared" si="3"/>
         <v>8.6493683242548419E-4</v>
       </c>
-      <c r="S22" s="109">
+      <c r="S22" s="107">
         <f t="shared" si="3"/>
         <v>8.6566058331098629E-4</v>
       </c>
-      <c r="T22" s="109">
+      <c r="T22" s="107">
         <f t="shared" si="3"/>
         <v>8.6623263602240346E-4</v>
       </c>
-      <c r="U22" s="109">
+      <c r="U22" s="107">
         <f t="shared" si="3"/>
         <v>8.6668678734664727E-4</v>
       </c>
-      <c r="V22" s="109">
+      <c r="V22" s="107">
         <f t="shared" si="3"/>
         <v>8.6704807354942234E-4</v>
       </c>
-      <c r="W22" s="109">
+      <c r="W22" s="107">
         <f t="shared" si="3"/>
         <v>8.6733554855185921E-4</v>
       </c>
-      <c r="X22" s="109">
+      <c r="X22" s="107">
         <f t="shared" si="3"/>
         <v>8.6756403355694176E-4</v>
       </c>
-      <c r="Y22" s="109">
+      <c r="Y22" s="107">
         <f t="shared" si="3"/>
         <v>8.6774467426508034E-4</v>
       </c>
-      <c r="Z22" s="109">
+      <c r="Z22" s="107">
         <f t="shared" si="3"/>
         <v>8.6788496129356892E-4</v>
       </c>
-      <c r="AA22" s="109">
+      <c r="AA22" s="107">
         <f t="shared" si="3"/>
         <v>8.679906435907829E-4</v>
       </c>
-      <c r="AB22" s="109">
+      <c r="AB22" s="107">
         <f t="shared" si="3"/>
         <v>8.6806703663604384E-4</v>
       </c>
-      <c r="AC22" s="109">
+      <c r="AC22" s="107">
         <f t="shared" si="3"/>
         <v>8.6812474931274419E-4</v>
       </c>
-      <c r="AD22" s="109">
+      <c r="AD22" s="107">
         <f t="shared" si="3"/>
         <v>8.6816656958161383E-4</v>
       </c>
-      <c r="AE22" s="109">
+      <c r="AE22" s="107">
         <f t="shared" si="3"/>
         <v>8.6819702409917938E-4</v>
       </c>
-      <c r="AF22" s="109">
+      <c r="AF22" s="107">
         <f t="shared" si="3"/>
         <v>8.682237041755898E-4</v>
       </c>
-      <c r="AG22" s="109">
+      <c r="AG22" s="107">
         <f t="shared" si="3"/>
         <v>8.6824712345240287E-4</v>
       </c>
-      <c r="AH22" s="109">
+      <c r="AH22" s="107">
         <f t="shared" si="3"/>
         <v>8.6826770417427362E-4</v>
       </c>
-      <c r="AI22" s="109">
+      <c r="AI22" s="107">
         <f t="shared" si="3"/>
         <v>8.6828585916602608E-4</v>
       </c>
-      <c r="AJ22" s="109">
+      <c r="AJ22" s="107">
         <f t="shared" si="3"/>
         <v>8.6830192616221846E-4</v>
       </c>
-      <c r="AK22" s="109">
+      <c r="AK22" s="107">
         <f t="shared" si="3"/>
         <v>8.6831619626461562E-4</v>
       </c>
-      <c r="AL22" s="109">
+      <c r="AL22" s="107">
         <f t="shared" si="3"/>
         <v>8.6832885780697565E-4</v>
       </c>
-      <c r="AM22" s="109">
+      <c r="AM22" s="107">
         <f t="shared" si="3"/>
         <v>8.6834012880109761E-4</v>
       </c>
-      <c r="AN22" s="109">
+      <c r="AN22" s="107">
         <f t="shared" si="3"/>
         <v>8.6835015705640493E-4</v>
       </c>
-      <c r="AO22" s="109">
+      <c r="AO22" s="107">
         <f t="shared" si="3"/>
         <v>8.6835907726930995E-4</v>
       </c>
-      <c r="AP22" s="109">
+      <c r="AP22" s="107">
         <f t="shared" si="3"/>
         <v>8.6836702418365127E-4</v>
       </c>
-      <c r="AQ22" s="109">
+      <c r="AQ22" s="107">
         <f t="shared" si="3"/>
         <v>8.6837412398812683E-4</v>
       </c>
-      <c r="AR22" s="109">
+      <c r="AR22" s="107">
         <f t="shared" si="3"/>
         <v>8.6838053018512495E-4</v>
       </c>
@@ -43001,7 +42966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -43165,7 +43130,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9823B3-B9A8-45BA-AB9B-6560A8BB5A72}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -45160,13 +45125,15 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:AK2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -45296,144 +45263,144 @@
         <v>1.2269199212468287E-3</v>
       </c>
       <c r="C2" s="9">
-        <f>C$4/(1-'Calculations Etc'!$B$3)</f>
+        <f>B2</f>
         <v>1.2269199212468287E-3</v>
       </c>
       <c r="D2" s="9">
-        <f>D$4/(1-'Calculations Etc'!$B$3)</f>
+        <f t="shared" ref="D2:AK2" si="0">C2</f>
         <v>1.2269199212468287E-3</v>
       </c>
-      <c r="E2" s="4">
-        <f>$D2+$D2*(E$1-$D$1)/($AK$1-$D$1)</f>
-        <v>1.264099312799763E-3</v>
-      </c>
-      <c r="F2" s="4">
-        <f t="shared" ref="F2:AK2" si="0">$D2+$D2*(F$1-$D$1)/($AK$1-$D$1)</f>
-        <v>1.3012787043526972E-3</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="E2" s="9">
         <f t="shared" si="0"/>
-        <v>1.3384580959056314E-3</v>
-      </c>
-      <c r="H2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="F2" s="9">
         <f t="shared" si="0"/>
-        <v>1.3756374874585656E-3</v>
-      </c>
-      <c r="I2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="G2" s="9">
         <f t="shared" si="0"/>
-        <v>1.4128168790114998E-3</v>
-      </c>
-      <c r="J2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="H2" s="9">
         <f t="shared" si="0"/>
-        <v>1.449996270564434E-3</v>
-      </c>
-      <c r="K2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="I2" s="9">
         <f t="shared" si="0"/>
-        <v>1.4871756621173682E-3</v>
-      </c>
-      <c r="L2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="J2" s="9">
         <f t="shared" si="0"/>
-        <v>1.5243550536703024E-3</v>
-      </c>
-      <c r="M2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="K2" s="9">
         <f t="shared" si="0"/>
-        <v>1.5615344452232366E-3</v>
-      </c>
-      <c r="N2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="L2" s="9">
         <f t="shared" si="0"/>
-        <v>1.5987138367761708E-3</v>
-      </c>
-      <c r="O2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="M2" s="9">
         <f t="shared" si="0"/>
-        <v>1.635893228329105E-3</v>
-      </c>
-      <c r="P2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="N2" s="9">
         <f t="shared" si="0"/>
-        <v>1.6730726198820392E-3</v>
-      </c>
-      <c r="Q2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="O2" s="9">
         <f t="shared" si="0"/>
-        <v>1.7102520114349734E-3</v>
-      </c>
-      <c r="R2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="P2" s="9">
         <f t="shared" si="0"/>
-        <v>1.7474314029879076E-3</v>
-      </c>
-      <c r="S2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="Q2" s="9">
         <f t="shared" si="0"/>
-        <v>1.7846107945408418E-3</v>
-      </c>
-      <c r="T2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="R2" s="9">
         <f t="shared" si="0"/>
-        <v>1.821790186093776E-3</v>
-      </c>
-      <c r="U2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="S2" s="9">
         <f t="shared" si="0"/>
-        <v>1.8589695776467102E-3</v>
-      </c>
-      <c r="V2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="T2" s="9">
         <f t="shared" si="0"/>
-        <v>1.8961489691996444E-3</v>
-      </c>
-      <c r="W2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="U2" s="9">
         <f t="shared" si="0"/>
-        <v>1.9333283607525786E-3</v>
-      </c>
-      <c r="X2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="V2" s="9">
         <f t="shared" si="0"/>
-        <v>1.9705077523055128E-3</v>
-      </c>
-      <c r="Y2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="W2" s="9">
         <f t="shared" si="0"/>
-        <v>2.007687143858447E-3</v>
-      </c>
-      <c r="Z2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="X2" s="9">
         <f t="shared" si="0"/>
-        <v>2.0448665354113812E-3</v>
-      </c>
-      <c r="AA2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="Y2" s="9">
         <f t="shared" si="0"/>
-        <v>2.0820459269643155E-3</v>
-      </c>
-      <c r="AB2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="Z2" s="9">
         <f t="shared" si="0"/>
-        <v>2.1192253185172497E-3</v>
-      </c>
-      <c r="AC2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AA2" s="9">
         <f t="shared" si="0"/>
-        <v>2.1564047100701839E-3</v>
-      </c>
-      <c r="AD2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AB2" s="9">
         <f t="shared" si="0"/>
-        <v>2.1935841016231181E-3</v>
-      </c>
-      <c r="AE2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AC2" s="9">
         <f t="shared" si="0"/>
-        <v>2.2307634931760523E-3</v>
-      </c>
-      <c r="AF2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AD2" s="9">
         <f t="shared" si="0"/>
-        <v>2.2679428847289865E-3</v>
-      </c>
-      <c r="AG2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AE2" s="9">
         <f t="shared" si="0"/>
-        <v>2.3051222762819207E-3</v>
-      </c>
-      <c r="AH2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AF2" s="9">
         <f t="shared" si="0"/>
-        <v>2.3423016678348549E-3</v>
-      </c>
-      <c r="AI2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AG2" s="9">
         <f t="shared" si="0"/>
-        <v>2.3794810593877891E-3</v>
-      </c>
-      <c r="AJ2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AH2" s="9">
         <f t="shared" si="0"/>
-        <v>2.4166604509407233E-3</v>
-      </c>
-      <c r="AK2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AI2" s="9">
         <f t="shared" si="0"/>
-        <v>2.4538398424936575E-3</v>
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AJ2" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AK2" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2269199212468287E-3</v>
       </c>
     </row>
     <row r="3" spans="1:37">
@@ -45901,135 +45868,135 @@
       </c>
       <c r="E6" s="4">
         <f>E4*(1-'Calculations Etc'!$B$8)+E2*'Calculations Etc'!$B$8</f>
-        <v>8.6864578446400832E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="F6" s="4">
         <f>F4*(1-'Calculations Etc'!$B$8)+F2*'Calculations Etc'!$B$8</f>
-        <v>8.890944498181222E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="G6" s="4">
         <f>G4*(1-'Calculations Etc'!$B$8)+G2*'Calculations Etc'!$B$8</f>
-        <v>9.0954311517223597E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="H6" s="4">
         <f>H4*(1-'Calculations Etc'!$B$8)+H2*'Calculations Etc'!$B$8</f>
-        <v>9.2999178052634974E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="I6" s="4">
         <f>I4*(1-'Calculations Etc'!$B$8)+I2*'Calculations Etc'!$B$8</f>
-        <v>9.5044044588046361E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="J6" s="4">
         <f>J4*(1-'Calculations Etc'!$B$8)+J2*'Calculations Etc'!$B$8</f>
-        <v>9.7088911123457738E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="K6" s="4">
         <f>K4*(1-'Calculations Etc'!$B$8)+K2*'Calculations Etc'!$B$8</f>
-        <v>9.9133777658869126E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="L6" s="4">
         <f>L4*(1-'Calculations Etc'!$B$8)+L2*'Calculations Etc'!$B$8</f>
-        <v>1.011786441942805E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="M6" s="4">
         <f>M4*(1-'Calculations Etc'!$B$8)+M2*'Calculations Etc'!$B$8</f>
-        <v>1.0322351072969188E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="N6" s="4">
         <f>N4*(1-'Calculations Etc'!$B$8)+N2*'Calculations Etc'!$B$8</f>
-        <v>1.0526837726510326E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="O6" s="4">
         <f>O4*(1-'Calculations Etc'!$B$8)+O2*'Calculations Etc'!$B$8</f>
-        <v>1.0731324380051463E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="P6" s="4">
         <f>P4*(1-'Calculations Etc'!$B$8)+P2*'Calculations Etc'!$B$8</f>
-        <v>1.0935811033592603E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="Q6" s="4">
         <f>Q4*(1-'Calculations Etc'!$B$8)+Q2*'Calculations Etc'!$B$8</f>
-        <v>1.1140297687133741E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="R6" s="4">
         <f>R4*(1-'Calculations Etc'!$B$8)+R2*'Calculations Etc'!$B$8</f>
-        <v>1.1344784340674879E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="S6" s="4">
         <f>S4*(1-'Calculations Etc'!$B$8)+S2*'Calculations Etc'!$B$8</f>
-        <v>1.1549270994216016E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="T6" s="4">
         <f>T4*(1-'Calculations Etc'!$B$8)+T2*'Calculations Etc'!$B$8</f>
-        <v>1.1753757647757154E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="U6" s="4">
         <f>U4*(1-'Calculations Etc'!$B$8)+U2*'Calculations Etc'!$B$8</f>
-        <v>1.1958244301298292E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="V6" s="4">
         <f>V4*(1-'Calculations Etc'!$B$8)+V2*'Calculations Etc'!$B$8</f>
-        <v>1.2162730954839432E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="W6" s="4">
         <f>W4*(1-'Calculations Etc'!$B$8)+W2*'Calculations Etc'!$B$8</f>
-        <v>1.2367217608380569E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="X6" s="4">
         <f>X4*(1-'Calculations Etc'!$B$8)+X2*'Calculations Etc'!$B$8</f>
-        <v>1.2571704261921707E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="Y6" s="4">
         <f>Y4*(1-'Calculations Etc'!$B$8)+Y2*'Calculations Etc'!$B$8</f>
-        <v>1.2776190915462845E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="Z6" s="4">
         <f>Z4*(1-'Calculations Etc'!$B$8)+Z2*'Calculations Etc'!$B$8</f>
-        <v>1.2980677569003982E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AA6" s="4">
         <f>AA4*(1-'Calculations Etc'!$B$8)+AA2*'Calculations Etc'!$B$8</f>
-        <v>1.3185164222545122E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AB6" s="4">
         <f>AB4*(1-'Calculations Etc'!$B$8)+AB2*'Calculations Etc'!$B$8</f>
-        <v>1.338965087608626E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AC6" s="4">
         <f>AC4*(1-'Calculations Etc'!$B$8)+AC2*'Calculations Etc'!$B$8</f>
-        <v>1.3594137529627398E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AD6" s="4">
         <f>AD4*(1-'Calculations Etc'!$B$8)+AD2*'Calculations Etc'!$B$8</f>
-        <v>1.3798624183168535E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AE6" s="4">
         <f>AE4*(1-'Calculations Etc'!$B$8)+AE2*'Calculations Etc'!$B$8</f>
-        <v>1.4003110836709673E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AF6" s="4">
         <f>AF4*(1-'Calculations Etc'!$B$8)+AF2*'Calculations Etc'!$B$8</f>
-        <v>1.4207597490250813E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AG6" s="4">
         <f>AG4*(1-'Calculations Etc'!$B$8)+AG2*'Calculations Etc'!$B$8</f>
-        <v>1.441208414379195E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AH6" s="4">
         <f>AH4*(1-'Calculations Etc'!$B$8)+AH2*'Calculations Etc'!$B$8</f>
-        <v>1.4616570797333088E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AI6" s="4">
         <f>AI4*(1-'Calculations Etc'!$B$8)+AI2*'Calculations Etc'!$B$8</f>
-        <v>1.4821057450874226E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AJ6" s="4">
         <f>AJ4*(1-'Calculations Etc'!$B$8)+AJ2*'Calculations Etc'!$B$8</f>
-        <v>1.5025544104415364E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AK6" s="4">
         <f>AK4*(1-'Calculations Etc'!$B$8)+AK2*'Calculations Etc'!$B$8</f>
-        <v>1.5230030757956503E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -46356,7 +46323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -47533,7 +47500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -48710,7 +48677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -49887,7 +49854,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -50010,7 +49977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -51042,7 +51009,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -52074,7 +52041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -53037,7 +53004,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -54069,7 +54036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -55032,7 +54999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -56068,7 +56035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -57255,7 +57222,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -58179,7 +58146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58303,7 +58270,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58438,7 +58405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58600,7 +58567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58762,7 +58729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58891,7 +58858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804A9106-3BA0-4B90-9845-AFCEFC0D7629}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Fixes to BNVFE and MPNVbT
</commit_message>
<xml_diff>
--- a/InputData/trans/BNVFE/BAU New Veh Fuel Economy.xlsx
+++ b/InputData/trans/BNVFE/BAU New Veh Fuel Economy.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\Brazil\Model\InputData\trans\BNVFE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\trans\BNVFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3D447C-C86A-4BE5-8409-D54692E1F7A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" firstSheet="21" activeTab="22" xr2:uid="{730F6D5A-6C3B-47E7-AA94-50A9B9E008D1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19395" windowHeight="10395" firstSheet="18" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -71,7 +70,7 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1258,7 +1257,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="12">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -2557,176 +2556,176 @@
     <xf numFmtId="9" fontId="0" fillId="40" borderId="0" xfId="153" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="34" borderId="0" xfId="153" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="40" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="40" borderId="26" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="40" borderId="0" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="29" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="40" borderId="26" xfId="155" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="156">
-    <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Body: normal cell 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Calculation 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Check Cell 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Column heading" xfId="36" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="8"/>
+    <cellStyle name="20% - Accent2 2" xfId="9"/>
+    <cellStyle name="20% - Accent3 2" xfId="10"/>
+    <cellStyle name="20% - Accent4 2" xfId="11"/>
+    <cellStyle name="20% - Accent5 2" xfId="12"/>
+    <cellStyle name="20% - Accent6 2" xfId="13"/>
+    <cellStyle name="40% - Accent1 2" xfId="14"/>
+    <cellStyle name="40% - Accent2 2" xfId="15"/>
+    <cellStyle name="40% - Accent3 2" xfId="16"/>
+    <cellStyle name="40% - Accent4 2" xfId="17"/>
+    <cellStyle name="40% - Accent5 2" xfId="18"/>
+    <cellStyle name="40% - Accent6 2" xfId="19"/>
+    <cellStyle name="60% - Accent1 2" xfId="20"/>
+    <cellStyle name="60% - Accent2 2" xfId="21"/>
+    <cellStyle name="60% - Accent3 2" xfId="22"/>
+    <cellStyle name="60% - Accent4 2" xfId="23"/>
+    <cellStyle name="60% - Accent5 2" xfId="24"/>
+    <cellStyle name="60% - Accent6 2" xfId="25"/>
+    <cellStyle name="Accent1 2" xfId="26"/>
+    <cellStyle name="Accent2 2" xfId="27"/>
+    <cellStyle name="Accent3 2" xfId="28"/>
+    <cellStyle name="Accent4 2" xfId="29"/>
+    <cellStyle name="Accent5 2" xfId="30"/>
+    <cellStyle name="Accent6 2" xfId="31"/>
+    <cellStyle name="Bad 2" xfId="32"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
+    <cellStyle name="Body: normal cell 2" xfId="33"/>
+    <cellStyle name="Calculation 2" xfId="34"/>
+    <cellStyle name="Check Cell 2" xfId="35"/>
+    <cellStyle name="Column heading" xfId="36"/>
     <cellStyle name="Comma" xfId="155" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="37" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Comma 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Comma 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Comma 4" xfId="40" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Comma 5" xfId="41" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Comma 6" xfId="42" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Comma 7" xfId="43" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Comma 8" xfId="44" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Corner heading" xfId="45" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Currency 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Currency 3" xfId="47" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Currency 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Data" xfId="49" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Data 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Data no deci" xfId="51" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Data Superscript" xfId="52" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="53" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Footnotes: top row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Good 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Header: bottom row 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Heading 1 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Heading 2 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Heading 3 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Heading 4 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Hed Side" xfId="63" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Hed Side 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Hed Side bold" xfId="65" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Hed Side Indent" xfId="66" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Hed Side Regular" xfId="67" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="68" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Hed Top" xfId="69" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Hed Top - SECTION" xfId="70" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Hed Top_3-new4" xfId="71" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="Comma 2" xfId="37"/>
+    <cellStyle name="Comma 2 2" xfId="38"/>
+    <cellStyle name="Comma 3" xfId="39"/>
+    <cellStyle name="Comma 4" xfId="40"/>
+    <cellStyle name="Comma 5" xfId="41"/>
+    <cellStyle name="Comma 6" xfId="42"/>
+    <cellStyle name="Comma 7" xfId="43"/>
+    <cellStyle name="Comma 8" xfId="44"/>
+    <cellStyle name="Corner heading" xfId="45"/>
+    <cellStyle name="Currency 2" xfId="46"/>
+    <cellStyle name="Currency 3" xfId="47"/>
+    <cellStyle name="Currency 3 2" xfId="48"/>
+    <cellStyle name="Data" xfId="49"/>
+    <cellStyle name="Data 2" xfId="50"/>
+    <cellStyle name="Data no deci" xfId="51"/>
+    <cellStyle name="Data Superscript" xfId="52"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="53"/>
+    <cellStyle name="Explanatory Text 2" xfId="54"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="55"/>
+    <cellStyle name="Footnotes: top row" xfId="2"/>
+    <cellStyle name="Footnotes: top row 2" xfId="56"/>
+    <cellStyle name="Good 2" xfId="57"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
+    <cellStyle name="Header: bottom row 2" xfId="58"/>
+    <cellStyle name="Heading 1 2" xfId="59"/>
+    <cellStyle name="Heading 2 2" xfId="60"/>
+    <cellStyle name="Heading 3 2" xfId="61"/>
+    <cellStyle name="Heading 4 2" xfId="62"/>
+    <cellStyle name="Hed Side" xfId="63"/>
+    <cellStyle name="Hed Side 2" xfId="64"/>
+    <cellStyle name="Hed Side bold" xfId="65"/>
+    <cellStyle name="Hed Side Indent" xfId="66"/>
+    <cellStyle name="Hed Side Regular" xfId="67"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="68"/>
+    <cellStyle name="Hed Top" xfId="69"/>
+    <cellStyle name="Hed Top - SECTION" xfId="70"/>
+    <cellStyle name="Hed Top_3-new4" xfId="71"/>
     <cellStyle name="Hyperlink" xfId="154" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Input 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="74" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Neutral 2" xfId="75" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="72"/>
+    <cellStyle name="Input 2" xfId="73"/>
+    <cellStyle name="Linked Cell 2" xfId="74"/>
+    <cellStyle name="Neutral 2" xfId="75"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="76" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 11" xfId="77" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Normal 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Normal 3" xfId="80" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Normal 3 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Normal 3 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="83" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Normal 3 2 3" xfId="84" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Normal 3 3" xfId="85" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Normal 3 3 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="87" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Normal 3 3 3" xfId="88" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Normal 3 4" xfId="89" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Normal 3 4 2" xfId="90" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Normal 3 5" xfId="91" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Normal 3 6" xfId="92" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Normal 3 7" xfId="93" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Normal 4" xfId="94" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Normal 4 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Normal 4 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Normal 4 2 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Normal 4 3" xfId="99" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Normal 4 3 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="101" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Normal 4 3 3" xfId="102" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Normal 4 4" xfId="103" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="Normal 4 4 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
-    <cellStyle name="Normal 4 5" xfId="105" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
-    <cellStyle name="Normal 4 6" xfId="106" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
-    <cellStyle name="Normal 4 7" xfId="107" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
-    <cellStyle name="Normal 5" xfId="108" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
-    <cellStyle name="Normal 5 2" xfId="109" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
-    <cellStyle name="Normal 5 3" xfId="110" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
-    <cellStyle name="Normal 6" xfId="111" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
-    <cellStyle name="Normal 6 2" xfId="112" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
-    <cellStyle name="Normal 7" xfId="113" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
-    <cellStyle name="Normal 7 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
-    <cellStyle name="Normal 8" xfId="115" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
-    <cellStyle name="Normal 9" xfId="116" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
-    <cellStyle name="Note 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
-    <cellStyle name="Note 2 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
-    <cellStyle name="Output 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
-    <cellStyle name="Parent row 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Normal 10" xfId="76"/>
+    <cellStyle name="Normal 11" xfId="77"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="78"/>
+    <cellStyle name="Normal 2 3" xfId="79"/>
+    <cellStyle name="Normal 3" xfId="80"/>
+    <cellStyle name="Normal 3 2" xfId="81"/>
+    <cellStyle name="Normal 3 2 2" xfId="82"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="83"/>
+    <cellStyle name="Normal 3 2 3" xfId="84"/>
+    <cellStyle name="Normal 3 3" xfId="85"/>
+    <cellStyle name="Normal 3 3 2" xfId="86"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="87"/>
+    <cellStyle name="Normal 3 3 3" xfId="88"/>
+    <cellStyle name="Normal 3 4" xfId="89"/>
+    <cellStyle name="Normal 3 4 2" xfId="90"/>
+    <cellStyle name="Normal 3 5" xfId="91"/>
+    <cellStyle name="Normal 3 6" xfId="92"/>
+    <cellStyle name="Normal 3 7" xfId="93"/>
+    <cellStyle name="Normal 4" xfId="94"/>
+    <cellStyle name="Normal 4 2" xfId="95"/>
+    <cellStyle name="Normal 4 2 2" xfId="96"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="97"/>
+    <cellStyle name="Normal 4 2 3" xfId="98"/>
+    <cellStyle name="Normal 4 3" xfId="99"/>
+    <cellStyle name="Normal 4 3 2" xfId="100"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="101"/>
+    <cellStyle name="Normal 4 3 3" xfId="102"/>
+    <cellStyle name="Normal 4 4" xfId="103"/>
+    <cellStyle name="Normal 4 4 2" xfId="104"/>
+    <cellStyle name="Normal 4 5" xfId="105"/>
+    <cellStyle name="Normal 4 6" xfId="106"/>
+    <cellStyle name="Normal 4 7" xfId="107"/>
+    <cellStyle name="Normal 5" xfId="108"/>
+    <cellStyle name="Normal 5 2" xfId="109"/>
+    <cellStyle name="Normal 5 3" xfId="110"/>
+    <cellStyle name="Normal 6" xfId="111"/>
+    <cellStyle name="Normal 6 2" xfId="112"/>
+    <cellStyle name="Normal 7" xfId="113"/>
+    <cellStyle name="Normal 7 2" xfId="114"/>
+    <cellStyle name="Normal 8" xfId="115"/>
+    <cellStyle name="Normal 9" xfId="116"/>
+    <cellStyle name="Note 2" xfId="117"/>
+    <cellStyle name="Note 2 2" xfId="118"/>
+    <cellStyle name="Output 2" xfId="119"/>
+    <cellStyle name="Parent row" xfId="3"/>
+    <cellStyle name="Parent row 2" xfId="120"/>
     <cellStyle name="Percent" xfId="153" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="121" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
-    <cellStyle name="Percent 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
-    <cellStyle name="Percent 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
-    <cellStyle name="Percent 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
-    <cellStyle name="Percent 4" xfId="125" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
-    <cellStyle name="Reference" xfId="126" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
-    <cellStyle name="Row heading" xfId="127" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
-    <cellStyle name="Source Hed" xfId="128" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
-    <cellStyle name="Source Letter" xfId="129" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
-    <cellStyle name="Source Superscript" xfId="130" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
-    <cellStyle name="Source Superscript 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
-    <cellStyle name="Source Text" xfId="132" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
-    <cellStyle name="Source Text 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
-    <cellStyle name="State" xfId="134" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
-    <cellStyle name="Superscript" xfId="135" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
-    <cellStyle name="Table Data" xfId="136" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
-    <cellStyle name="Table Head Top" xfId="137" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
-    <cellStyle name="Table Hed Side" xfId="138" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
-    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
-    <cellStyle name="Table title 2" xfId="139" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
-    <cellStyle name="Title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
-    <cellStyle name="Title Text" xfId="141" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
-    <cellStyle name="Title Text 1" xfId="142" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
-    <cellStyle name="Title Text 2" xfId="143" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
-    <cellStyle name="Title-1" xfId="144" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
-    <cellStyle name="Title-2" xfId="145" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
-    <cellStyle name="Title-3" xfId="146" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
-    <cellStyle name="Total 2" xfId="147" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
-    <cellStyle name="Warning Text 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
-    <cellStyle name="Wrap" xfId="149" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
-    <cellStyle name="Wrap Bold" xfId="150" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
-    <cellStyle name="Wrap Title" xfId="151" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="152" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="Percent 2" xfId="121"/>
+    <cellStyle name="Percent 2 2" xfId="122"/>
+    <cellStyle name="Percent 3" xfId="123"/>
+    <cellStyle name="Percent 3 2" xfId="124"/>
+    <cellStyle name="Percent 4" xfId="125"/>
+    <cellStyle name="Reference" xfId="126"/>
+    <cellStyle name="Row heading" xfId="127"/>
+    <cellStyle name="Source Hed" xfId="128"/>
+    <cellStyle name="Source Letter" xfId="129"/>
+    <cellStyle name="Source Superscript" xfId="130"/>
+    <cellStyle name="Source Superscript 2" xfId="131"/>
+    <cellStyle name="Source Text" xfId="132"/>
+    <cellStyle name="Source Text 2" xfId="133"/>
+    <cellStyle name="State" xfId="134"/>
+    <cellStyle name="Superscript" xfId="135"/>
+    <cellStyle name="Table Data" xfId="136"/>
+    <cellStyle name="Table Head Top" xfId="137"/>
+    <cellStyle name="Table Hed Side" xfId="138"/>
+    <cellStyle name="Table title" xfId="7"/>
+    <cellStyle name="Table title 2" xfId="139"/>
+    <cellStyle name="Title 2" xfId="140"/>
+    <cellStyle name="Title Text" xfId="141"/>
+    <cellStyle name="Title Text 1" xfId="142"/>
+    <cellStyle name="Title Text 2" xfId="143"/>
+    <cellStyle name="Title-1" xfId="144"/>
+    <cellStyle name="Title-2" xfId="145"/>
+    <cellStyle name="Title-3" xfId="146"/>
+    <cellStyle name="Total 2" xfId="147"/>
+    <cellStyle name="Warning Text 2" xfId="148"/>
+    <cellStyle name="Wrap" xfId="149"/>
+    <cellStyle name="Wrap Bold" xfId="150"/>
+    <cellStyle name="Wrap Title" xfId="151"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="152"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3542,23 +3541,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3594,23 +3576,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3786,7 +3751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD190"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37341,15 +37306,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B63" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B26" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B34" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B48" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B56" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B41" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B78" r:id="rId9" xr:uid="{88250872-3BE8-4809-AAF6-4E90E919070B}"/>
+    <hyperlink ref="B63" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B17" r:id="rId3"/>
+    <hyperlink ref="B26" r:id="rId4"/>
+    <hyperlink ref="B34" r:id="rId5"/>
+    <hyperlink ref="B48" r:id="rId6"/>
+    <hyperlink ref="B56" r:id="rId7"/>
+    <hyperlink ref="B41" r:id="rId8"/>
+    <hyperlink ref="B78" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -37357,7 +37322,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37561,7 +37526,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37611,7 +37576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37641,7 +37606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37690,7 +37655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37805,7 +37770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37907,7 +37872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38069,7 +38034,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38215,7 +38180,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38289,7 +38254,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -38387,40 +38352,40 @@
       <c r="H13" s="39"/>
     </row>
     <row r="14" spans="1:14" ht="21">
-      <c r="A14" s="105" t="s">
+      <c r="A14" s="111" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="105"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="105"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="105"/>
-      <c r="N14" s="105"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="111"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
+      <c r="K14" s="111"/>
+      <c r="L14" s="111"/>
+      <c r="M14" s="111"/>
+      <c r="N14" s="111"/>
     </row>
     <row r="15" spans="1:14" ht="16.149999999999999" thickBot="1">
-      <c r="A15" s="106" t="s">
+      <c r="A15" s="112" t="s">
         <v>243</v>
       </c>
-      <c r="B15" s="106"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="106"/>
-      <c r="M15" s="106"/>
-      <c r="N15" s="106"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="112"/>
     </row>
     <row r="16" spans="1:14" ht="14.65" thickBot="1">
       <c r="A16" s="43"/>
@@ -40796,14 +40761,14 @@
     <mergeCell ref="A15:N15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I8" r:id="rId1" xr:uid="{90B25065-98AF-40EC-9EC5-C549B8D2D7C0}"/>
+    <hyperlink ref="I8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -40959,8 +40924,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D18" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D19" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D18" r:id="rId1"/>
+    <hyperlink ref="D19" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -40968,7 +40933,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -41023,7 +40988,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="A4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -41031,7 +40996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780079A6-729A-4BF6-A60D-8613DB4EC2FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -41044,7 +41009,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -41125,11 +41090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -41688,7 +41653,7 @@
       <c r="F11">
         <v>8.7048677754535786E-2</v>
       </c>
-      <c r="I11" s="107" t="s">
+      <c r="I11" s="105" t="s">
         <v>384</v>
       </c>
     </row>
@@ -42182,139 +42147,139 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="K16" s="108">
+      <c r="K16" s="106">
         <f>SUM(K13:K15)</f>
         <v>120062285703208.23</v>
       </c>
-      <c r="L16" s="108">
+      <c r="L16" s="106">
         <f t="shared" ref="L16:AR16" si="0">SUM(L13:L15)</f>
         <v>125222436550851.09</v>
       </c>
-      <c r="M16" s="108">
+      <c r="M16" s="106">
         <f t="shared" si="0"/>
         <v>130841787410825.59</v>
       </c>
-      <c r="N16" s="108">
+      <c r="N16" s="106">
         <f t="shared" si="0"/>
         <v>136954936909647.2</v>
       </c>
-      <c r="O16" s="108">
+      <c r="O16" s="106">
         <f t="shared" si="0"/>
         <v>143651317601530.53</v>
       </c>
-      <c r="P16" s="108">
+      <c r="P16" s="106">
         <f t="shared" si="0"/>
         <v>150985989668157</v>
       </c>
-      <c r="Q16" s="108">
+      <c r="Q16" s="106">
         <f t="shared" si="0"/>
         <v>158980245644967.91</v>
       </c>
-      <c r="R16" s="108">
+      <c r="R16" s="106">
         <f t="shared" si="0"/>
         <v>167612909015385.47</v>
       </c>
-      <c r="S16" s="108">
+      <c r="S16" s="106">
         <f t="shared" si="0"/>
         <v>176226946308777.75</v>
       </c>
-      <c r="T16" s="108">
+      <c r="T16" s="106">
         <f t="shared" si="0"/>
         <v>184273479514302.25</v>
       </c>
-      <c r="U16" s="108">
+      <c r="U16" s="106">
         <f t="shared" si="0"/>
         <v>191799878334263.22</v>
       </c>
-      <c r="V16" s="108">
+      <c r="V16" s="106">
         <f t="shared" si="0"/>
         <v>198838374046822.38</v>
       </c>
-      <c r="W16" s="108">
+      <c r="W16" s="106">
         <f t="shared" si="0"/>
         <v>205419107525463</v>
       </c>
-      <c r="X16" s="108">
+      <c r="X16" s="106">
         <f t="shared" si="0"/>
         <v>211570277896100</v>
       </c>
-      <c r="Y16" s="108">
+      <c r="Y16" s="106">
         <f t="shared" si="0"/>
         <v>217336000393173.84</v>
       </c>
-      <c r="Z16" s="108">
+      <c r="Z16" s="106">
         <f t="shared" si="0"/>
         <v>222755892217345.38</v>
       </c>
-      <c r="AA16" s="108">
+      <c r="AA16" s="106">
         <f t="shared" si="0"/>
         <v>227862150680357.19</v>
       </c>
-      <c r="AB16" s="108">
+      <c r="AB16" s="106">
         <f t="shared" si="0"/>
         <v>232691363772114.59</v>
       </c>
-      <c r="AC16" s="108">
+      <c r="AC16" s="106">
         <f t="shared" si="0"/>
         <v>237102223499737.22</v>
       </c>
-      <c r="AD16" s="108">
+      <c r="AD16" s="106">
         <f t="shared" si="0"/>
         <v>241017198099816.56</v>
       </c>
-      <c r="AE16" s="108">
+      <c r="AE16" s="106">
         <f t="shared" si="0"/>
         <v>244497221223826.41</v>
       </c>
-      <c r="AF16" s="108">
+      <c r="AF16" s="106">
         <f t="shared" si="0"/>
         <v>247574100504740.09</v>
       </c>
-      <c r="AG16" s="108">
+      <c r="AG16" s="106">
         <f t="shared" si="0"/>
         <v>250293751878965</v>
       </c>
-      <c r="AH16" s="108">
+      <c r="AH16" s="106">
         <f t="shared" si="0"/>
         <v>252696972462987.28</v>
       </c>
-      <c r="AI16" s="108">
+      <c r="AI16" s="106">
         <f t="shared" si="0"/>
         <v>254822131381383.34</v>
       </c>
-      <c r="AJ16" s="108">
+      <c r="AJ16" s="106">
         <f t="shared" si="0"/>
         <v>256704382678802.69</v>
       </c>
-      <c r="AK16" s="108">
+      <c r="AK16" s="106">
         <f t="shared" si="0"/>
         <v>258374696279324.5</v>
       </c>
-      <c r="AL16" s="108">
+      <c r="AL16" s="106">
         <f t="shared" si="0"/>
         <v>259862086903347.5</v>
       </c>
-      <c r="AM16" s="108">
+      <c r="AM16" s="106">
         <f t="shared" si="0"/>
         <v>261191839526366.16</v>
       </c>
-      <c r="AN16" s="108">
+      <c r="AN16" s="106">
         <f t="shared" si="0"/>
         <v>262388277951264.31</v>
       </c>
-      <c r="AO16" s="108">
+      <c r="AO16" s="106">
         <f t="shared" si="0"/>
         <v>263473146983350.19</v>
       </c>
-      <c r="AP16" s="108">
+      <c r="AP16" s="106">
         <f t="shared" si="0"/>
         <v>264464945107297.25</v>
       </c>
-      <c r="AQ16" s="108">
+      <c r="AQ16" s="106">
         <f t="shared" si="0"/>
         <v>265379784616347.31</v>
       </c>
-      <c r="AR16" s="108">
+      <c r="AR16" s="106">
         <f t="shared" si="0"/>
         <v>266231285184595.69</v>
       </c>
@@ -42436,139 +42401,139 @@
       <c r="I19" t="s">
         <v>387</v>
       </c>
-      <c r="K19" s="111">
+      <c r="K19" s="109">
         <f>K18*10^3</f>
         <v>164878851200</v>
       </c>
-      <c r="L19" s="111">
+      <c r="L19" s="109">
         <f t="shared" ref="L19:AR19" si="1">L18*10^3</f>
         <v>172476613600.00003</v>
       </c>
-      <c r="M19" s="111">
+      <c r="M19" s="109">
         <f t="shared" si="1"/>
         <v>180682556000</v>
       </c>
-      <c r="N19" s="111">
+      <c r="N19" s="109">
         <f t="shared" si="1"/>
         <v>189542353200</v>
       </c>
-      <c r="O19" s="111">
+      <c r="O19" s="109">
         <f t="shared" si="1"/>
         <v>199181827200</v>
       </c>
-      <c r="P19" s="111">
+      <c r="P19" s="109">
         <f t="shared" si="1"/>
         <v>209680173600.00003</v>
       </c>
-      <c r="Q19" s="111">
+      <c r="Q19" s="109">
         <f t="shared" si="1"/>
         <v>221066006399.99997</v>
       </c>
-      <c r="R19" s="111">
+      <c r="R19" s="109">
         <f t="shared" si="1"/>
         <v>233314040400</v>
       </c>
-      <c r="S19" s="111">
+      <c r="S19" s="109">
         <f t="shared" si="1"/>
         <v>245509882400</v>
       </c>
-      <c r="T19" s="111">
+      <c r="T19" s="109">
         <f t="shared" si="1"/>
         <v>256889526400</v>
       </c>
-      <c r="U19" s="111">
+      <c r="U19" s="109">
         <f t="shared" si="1"/>
         <v>267522012400</v>
       </c>
-      <c r="V19" s="111">
+      <c r="V19" s="109">
         <f t="shared" si="1"/>
         <v>277454900800</v>
       </c>
-      <c r="W19" s="111">
+      <c r="W19" s="109">
         <f t="shared" si="1"/>
         <v>286732554800</v>
       </c>
-      <c r="X19" s="111">
+      <c r="X19" s="109">
         <f t="shared" si="1"/>
         <v>295396411600</v>
       </c>
-      <c r="Y19" s="111">
+      <c r="Y19" s="109">
         <f t="shared" si="1"/>
         <v>303509750000</v>
       </c>
-      <c r="Z19" s="111">
+      <c r="Z19" s="109">
         <f t="shared" si="1"/>
         <v>311128921200</v>
       </c>
-      <c r="AA19" s="111">
+      <c r="AA19" s="109">
         <f t="shared" si="1"/>
         <v>318299719200</v>
       </c>
-      <c r="AB19" s="111">
+      <c r="AB19" s="109">
         <f t="shared" si="1"/>
         <v>325074235200</v>
       </c>
-      <c r="AC19" s="111">
+      <c r="AC19" s="109">
         <f t="shared" si="1"/>
         <v>331258311600</v>
       </c>
-      <c r="AD19" s="111">
+      <c r="AD19" s="109">
         <f t="shared" si="1"/>
         <v>336744190000</v>
       </c>
-      <c r="AE19" s="111">
+      <c r="AE19" s="109">
         <f t="shared" si="1"/>
         <v>341618388800</v>
       </c>
-      <c r="AF19" s="111">
+      <c r="AF19" s="109">
         <f t="shared" si="1"/>
         <v>345928121200</v>
       </c>
-      <c r="AG19" s="111">
+      <c r="AG19" s="109">
         <f t="shared" si="1"/>
         <v>349737644800</v>
       </c>
-      <c r="AH19" s="111">
+      <c r="AH19" s="109">
         <f t="shared" si="1"/>
         <v>353104055600</v>
       </c>
-      <c r="AI19" s="111">
+      <c r="AI19" s="109">
         <f t="shared" si="1"/>
         <v>356081074400</v>
       </c>
-      <c r="AJ19" s="111">
+      <c r="AJ19" s="109">
         <f t="shared" si="1"/>
         <v>358717915600</v>
       </c>
-      <c r="AK19" s="111">
+      <c r="AK19" s="109">
         <f t="shared" si="1"/>
         <v>361057940400</v>
       </c>
-      <c r="AL19" s="111">
+      <c r="AL19" s="109">
         <f t="shared" si="1"/>
         <v>363141744800</v>
       </c>
-      <c r="AM19" s="111">
+      <c r="AM19" s="109">
         <f t="shared" si="1"/>
         <v>365004732400</v>
       </c>
-      <c r="AN19" s="111">
+      <c r="AN19" s="109">
         <f t="shared" si="1"/>
         <v>366680940000</v>
       </c>
-      <c r="AO19" s="111">
+      <c r="AO19" s="109">
         <f t="shared" si="1"/>
         <v>368200799200.00006</v>
       </c>
-      <c r="AP19" s="111">
+      <c r="AP19" s="109">
         <f t="shared" si="1"/>
         <v>369590208400</v>
       </c>
-      <c r="AQ19" s="111">
+      <c r="AQ19" s="109">
         <f t="shared" si="1"/>
         <v>370871730400</v>
       </c>
-      <c r="AR19" s="111">
+      <c r="AR19" s="109">
         <f t="shared" si="1"/>
         <v>372064458400</v>
       </c>
@@ -42577,139 +42542,139 @@
       <c r="I20" t="s">
         <v>385</v>
       </c>
-      <c r="K20" s="110">
+      <c r="K20" s="108">
         <f>K19*units_convertor!$A$2</f>
         <v>102450936648.99519</v>
       </c>
-      <c r="L20" s="110">
+      <c r="L20" s="108">
         <f>L19*units_convertor!$A$2</f>
         <v>107171965869.24562</v>
       </c>
-      <c r="M20" s="110">
+      <c r="M20" s="108">
         <f>M19*units_convertor!$A$2</f>
         <v>112270900504.276</v>
       </c>
-      <c r="N20" s="110">
+      <c r="N20" s="108">
         <f>N19*units_convertor!$A$2</f>
         <v>117776121550.2372</v>
       </c>
-      <c r="O20" s="110">
+      <c r="O20" s="108">
         <f>O19*units_convertor!$A$2</f>
         <v>123765811149.0912</v>
       </c>
-      <c r="P20" s="110">
+      <c r="P20" s="108">
         <f>P19*units_convertor!$A$2</f>
         <v>130289179150.00562</v>
       </c>
-      <c r="Q20" s="110">
+      <c r="Q20" s="108">
         <f>Q19*units_convertor!$A$2</f>
         <v>137364005462.77438</v>
       </c>
-      <c r="R20" s="110">
+      <c r="R20" s="108">
         <f>R19*units_convertor!$A$2</f>
         <v>144974578597.3884</v>
       </c>
-      <c r="S20" s="110">
+      <c r="S20" s="108">
         <f>S19*units_convertor!$A$2</f>
         <v>152552721136.77042</v>
       </c>
-      <c r="T20" s="110">
+      <c r="T20" s="108">
         <f>T19*units_convertor!$A$2</f>
         <v>159623701908.6944</v>
       </c>
-      <c r="U20" s="110">
+      <c r="U20" s="108">
         <f>U19*units_convertor!$A$2</f>
         <v>166230420367.0004</v>
       </c>
-      <c r="V20" s="110">
+      <c r="V20" s="108">
         <f>V19*units_convertor!$A$2</f>
         <v>172402429164.9968</v>
       </c>
-      <c r="W20" s="110">
+      <c r="W20" s="108">
         <f>W19*units_convertor!$A$2</f>
         <v>178167294308.6308</v>
       </c>
-      <c r="X20" s="110">
+      <c r="X20" s="108">
         <f>X19*units_convertor!$A$2</f>
         <v>183550763672.30359</v>
       </c>
-      <c r="Y20" s="110">
+      <c r="Y20" s="108">
         <f>Y19*units_convertor!$A$2</f>
         <v>188592156867.25</v>
       </c>
-      <c r="Z20" s="110">
+      <c r="Z20" s="108">
         <f>Z19*units_convertor!$A$2</f>
         <v>193326488894.96521</v>
       </c>
-      <c r="AA20" s="110">
+      <c r="AA20" s="108">
         <f>AA19*units_convertor!$A$2</f>
         <v>197782214819.02319</v>
       </c>
-      <c r="AB20" s="110">
+      <c r="AB20" s="108">
         <f>AB19*units_convertor!$A$2</f>
         <v>201991702600.4592</v>
       </c>
-      <c r="AC20" s="110">
+      <c r="AC20" s="108">
         <f>AC19*units_convertor!$A$2</f>
         <v>205834308337.20361</v>
       </c>
-      <c r="AD20" s="110">
+      <c r="AD20" s="108">
         <f>AD19*units_convertor!$A$2</f>
         <v>209243074084.48999</v>
       </c>
-      <c r="AE20" s="110">
+      <c r="AE20" s="108">
         <f>AE19*units_convertor!$A$2</f>
         <v>212271759867.0448</v>
       </c>
-      <c r="AF20" s="110">
+      <c r="AF20" s="108">
         <f>AF19*units_convertor!$A$2</f>
         <v>214949702598.16519</v>
       </c>
-      <c r="AG20" s="110">
+      <c r="AG20" s="108">
         <f>AG19*units_convertor!$A$2</f>
         <v>217316830087.02081</v>
       </c>
-      <c r="AH20" s="110">
+      <c r="AH20" s="108">
         <f>AH19*units_convertor!$A$2</f>
         <v>219408620132.2276</v>
       </c>
-      <c r="AI20" s="110">
+      <c r="AI20" s="108">
         <f>AI19*units_convertor!$A$2</f>
         <v>221258453281.00241</v>
       </c>
-      <c r="AJ20" s="110">
+      <c r="AJ20" s="108">
         <f>AJ19*units_convertor!$A$2</f>
         <v>222896909934.2876</v>
       </c>
-      <c r="AK20" s="110">
+      <c r="AK20" s="108">
         <f>AK19*units_convertor!$A$2</f>
         <v>224350933484.28839</v>
       </c>
-      <c r="AL20" s="110">
+      <c r="AL20" s="108">
         <f>AL19*units_convertor!$A$2</f>
         <v>225645749108.12079</v>
       </c>
-      <c r="AM20" s="110">
+      <c r="AM20" s="108">
         <f>AM19*units_convertor!$A$2</f>
         <v>226803355576.12039</v>
       </c>
-      <c r="AN20" s="110">
+      <c r="AN20" s="108">
         <f>AN19*units_convertor!$A$2</f>
         <v>227844902368.73999</v>
       </c>
-      <c r="AO20" s="110">
+      <c r="AO20" s="108">
         <f>AO19*units_convertor!$A$2</f>
         <v>228789298799.70325</v>
       </c>
-      <c r="AP20" s="110">
+      <c r="AP20" s="108">
         <f>AP19*units_convertor!$A$2</f>
         <v>229652637383.7164</v>
       </c>
-      <c r="AQ20" s="110">
+      <c r="AQ20" s="108">
         <f>AQ19*units_convertor!$A$2</f>
         <v>230448937990.37839</v>
       </c>
-      <c r="AR20" s="110">
+      <c r="AR20" s="108">
         <f>AR19*units_convertor!$A$2</f>
         <v>231190064580.4664</v>
       </c>
@@ -42857,139 +42822,139 @@
       <c r="I22" t="s">
         <v>386</v>
       </c>
-      <c r="K22" s="112">
+      <c r="K22" s="110">
         <f>K20/K16</f>
         <v>8.5331489442281672E-4</v>
       </c>
-      <c r="L22" s="109">
+      <c r="L22" s="107">
         <f t="shared" ref="L22:AR22" si="3">L20/L16</f>
         <v>8.5585274349556822E-4</v>
       </c>
-      <c r="M22" s="109">
+      <c r="M22" s="107">
         <f t="shared" si="3"/>
         <v>8.5806608672931448E-4</v>
       </c>
-      <c r="N22" s="109">
+      <c r="N22" s="107">
         <f t="shared" si="3"/>
         <v>8.5996258483136848E-4</v>
       </c>
-      <c r="O22" s="109">
+      <c r="O22" s="107">
         <f t="shared" si="3"/>
         <v>8.6157101247341802E-4</v>
       </c>
-      <c r="P22" s="109">
+      <c r="P22" s="107">
         <f t="shared" si="3"/>
         <v>8.62922311112179E-4</v>
       </c>
-      <c r="Q22" s="109">
+      <c r="Q22" s="107">
         <f t="shared" si="3"/>
         <v>8.6403191104342258E-4</v>
       </c>
-      <c r="R22" s="109">
+      <c r="R22" s="107">
         <f t="shared" si="3"/>
         <v>8.6493683242548419E-4</v>
       </c>
-      <c r="S22" s="109">
+      <c r="S22" s="107">
         <f t="shared" si="3"/>
         <v>8.6566058331098629E-4</v>
       </c>
-      <c r="T22" s="109">
+      <c r="T22" s="107">
         <f t="shared" si="3"/>
         <v>8.6623263602240346E-4</v>
       </c>
-      <c r="U22" s="109">
+      <c r="U22" s="107">
         <f t="shared" si="3"/>
         <v>8.6668678734664727E-4</v>
       </c>
-      <c r="V22" s="109">
+      <c r="V22" s="107">
         <f t="shared" si="3"/>
         <v>8.6704807354942234E-4</v>
       </c>
-      <c r="W22" s="109">
+      <c r="W22" s="107">
         <f t="shared" si="3"/>
         <v>8.6733554855185921E-4</v>
       </c>
-      <c r="X22" s="109">
+      <c r="X22" s="107">
         <f t="shared" si="3"/>
         <v>8.6756403355694176E-4</v>
       </c>
-      <c r="Y22" s="109">
+      <c r="Y22" s="107">
         <f t="shared" si="3"/>
         <v>8.6774467426508034E-4</v>
       </c>
-      <c r="Z22" s="109">
+      <c r="Z22" s="107">
         <f t="shared" si="3"/>
         <v>8.6788496129356892E-4</v>
       </c>
-      <c r="AA22" s="109">
+      <c r="AA22" s="107">
         <f t="shared" si="3"/>
         <v>8.679906435907829E-4</v>
       </c>
-      <c r="AB22" s="109">
+      <c r="AB22" s="107">
         <f t="shared" si="3"/>
         <v>8.6806703663604384E-4</v>
       </c>
-      <c r="AC22" s="109">
+      <c r="AC22" s="107">
         <f t="shared" si="3"/>
         <v>8.6812474931274419E-4</v>
       </c>
-      <c r="AD22" s="109">
+      <c r="AD22" s="107">
         <f t="shared" si="3"/>
         <v>8.6816656958161383E-4</v>
       </c>
-      <c r="AE22" s="109">
+      <c r="AE22" s="107">
         <f t="shared" si="3"/>
         <v>8.6819702409917938E-4</v>
       </c>
-      <c r="AF22" s="109">
+      <c r="AF22" s="107">
         <f t="shared" si="3"/>
         <v>8.682237041755898E-4</v>
       </c>
-      <c r="AG22" s="109">
+      <c r="AG22" s="107">
         <f t="shared" si="3"/>
         <v>8.6824712345240287E-4</v>
       </c>
-      <c r="AH22" s="109">
+      <c r="AH22" s="107">
         <f t="shared" si="3"/>
         <v>8.6826770417427362E-4</v>
       </c>
-      <c r="AI22" s="109">
+      <c r="AI22" s="107">
         <f t="shared" si="3"/>
         <v>8.6828585916602608E-4</v>
       </c>
-      <c r="AJ22" s="109">
+      <c r="AJ22" s="107">
         <f t="shared" si="3"/>
         <v>8.6830192616221846E-4</v>
       </c>
-      <c r="AK22" s="109">
+      <c r="AK22" s="107">
         <f t="shared" si="3"/>
         <v>8.6831619626461562E-4</v>
       </c>
-      <c r="AL22" s="109">
+      <c r="AL22" s="107">
         <f t="shared" si="3"/>
         <v>8.6832885780697565E-4</v>
       </c>
-      <c r="AM22" s="109">
+      <c r="AM22" s="107">
         <f t="shared" si="3"/>
         <v>8.6834012880109761E-4</v>
       </c>
-      <c r="AN22" s="109">
+      <c r="AN22" s="107">
         <f t="shared" si="3"/>
         <v>8.6835015705640493E-4</v>
       </c>
-      <c r="AO22" s="109">
+      <c r="AO22" s="107">
         <f t="shared" si="3"/>
         <v>8.6835907726930995E-4</v>
       </c>
-      <c r="AP22" s="109">
+      <c r="AP22" s="107">
         <f t="shared" si="3"/>
         <v>8.6836702418365127E-4</v>
       </c>
-      <c r="AQ22" s="109">
+      <c r="AQ22" s="107">
         <f t="shared" si="3"/>
         <v>8.6837412398812683E-4</v>
       </c>
-      <c r="AR22" s="109">
+      <c r="AR22" s="107">
         <f t="shared" si="3"/>
         <v>8.6838053018512495E-4</v>
       </c>
@@ -43001,7 +42966,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -43165,7 +43130,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9823B3-B9A8-45BA-AB9B-6560A8BB5A72}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -45160,13 +45125,15 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:AK2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -45296,144 +45263,144 @@
         <v>1.2269199212468287E-3</v>
       </c>
       <c r="C2" s="9">
-        <f>C$4/(1-'Calculations Etc'!$B$3)</f>
+        <f>B2</f>
         <v>1.2269199212468287E-3</v>
       </c>
       <c r="D2" s="9">
-        <f>D$4/(1-'Calculations Etc'!$B$3)</f>
+        <f t="shared" ref="D2:AK2" si="0">C2</f>
         <v>1.2269199212468287E-3</v>
       </c>
-      <c r="E2" s="4">
-        <f>$D2+$D2*(E$1-$D$1)/($AK$1-$D$1)</f>
-        <v>1.264099312799763E-3</v>
-      </c>
-      <c r="F2" s="4">
-        <f t="shared" ref="F2:AK2" si="0">$D2+$D2*(F$1-$D$1)/($AK$1-$D$1)</f>
-        <v>1.3012787043526972E-3</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="E2" s="9">
         <f t="shared" si="0"/>
-        <v>1.3384580959056314E-3</v>
-      </c>
-      <c r="H2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="F2" s="9">
         <f t="shared" si="0"/>
-        <v>1.3756374874585656E-3</v>
-      </c>
-      <c r="I2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="G2" s="9">
         <f t="shared" si="0"/>
-        <v>1.4128168790114998E-3</v>
-      </c>
-      <c r="J2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="H2" s="9">
         <f t="shared" si="0"/>
-        <v>1.449996270564434E-3</v>
-      </c>
-      <c r="K2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="I2" s="9">
         <f t="shared" si="0"/>
-        <v>1.4871756621173682E-3</v>
-      </c>
-      <c r="L2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="J2" s="9">
         <f t="shared" si="0"/>
-        <v>1.5243550536703024E-3</v>
-      </c>
-      <c r="M2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="K2" s="9">
         <f t="shared" si="0"/>
-        <v>1.5615344452232366E-3</v>
-      </c>
-      <c r="N2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="L2" s="9">
         <f t="shared" si="0"/>
-        <v>1.5987138367761708E-3</v>
-      </c>
-      <c r="O2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="M2" s="9">
         <f t="shared" si="0"/>
-        <v>1.635893228329105E-3</v>
-      </c>
-      <c r="P2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="N2" s="9">
         <f t="shared" si="0"/>
-        <v>1.6730726198820392E-3</v>
-      </c>
-      <c r="Q2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="O2" s="9">
         <f t="shared" si="0"/>
-        <v>1.7102520114349734E-3</v>
-      </c>
-      <c r="R2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="P2" s="9">
         <f t="shared" si="0"/>
-        <v>1.7474314029879076E-3</v>
-      </c>
-      <c r="S2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="Q2" s="9">
         <f t="shared" si="0"/>
-        <v>1.7846107945408418E-3</v>
-      </c>
-      <c r="T2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="R2" s="9">
         <f t="shared" si="0"/>
-        <v>1.821790186093776E-3</v>
-      </c>
-      <c r="U2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="S2" s="9">
         <f t="shared" si="0"/>
-        <v>1.8589695776467102E-3</v>
-      </c>
-      <c r="V2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="T2" s="9">
         <f t="shared" si="0"/>
-        <v>1.8961489691996444E-3</v>
-      </c>
-      <c r="W2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="U2" s="9">
         <f t="shared" si="0"/>
-        <v>1.9333283607525786E-3</v>
-      </c>
-      <c r="X2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="V2" s="9">
         <f t="shared" si="0"/>
-        <v>1.9705077523055128E-3</v>
-      </c>
-      <c r="Y2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="W2" s="9">
         <f t="shared" si="0"/>
-        <v>2.007687143858447E-3</v>
-      </c>
-      <c r="Z2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="X2" s="9">
         <f t="shared" si="0"/>
-        <v>2.0448665354113812E-3</v>
-      </c>
-      <c r="AA2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="Y2" s="9">
         <f t="shared" si="0"/>
-        <v>2.0820459269643155E-3</v>
-      </c>
-      <c r="AB2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="Z2" s="9">
         <f t="shared" si="0"/>
-        <v>2.1192253185172497E-3</v>
-      </c>
-      <c r="AC2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AA2" s="9">
         <f t="shared" si="0"/>
-        <v>2.1564047100701839E-3</v>
-      </c>
-      <c r="AD2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AB2" s="9">
         <f t="shared" si="0"/>
-        <v>2.1935841016231181E-3</v>
-      </c>
-      <c r="AE2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AC2" s="9">
         <f t="shared" si="0"/>
-        <v>2.2307634931760523E-3</v>
-      </c>
-      <c r="AF2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AD2" s="9">
         <f t="shared" si="0"/>
-        <v>2.2679428847289865E-3</v>
-      </c>
-      <c r="AG2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AE2" s="9">
         <f t="shared" si="0"/>
-        <v>2.3051222762819207E-3</v>
-      </c>
-      <c r="AH2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AF2" s="9">
         <f t="shared" si="0"/>
-        <v>2.3423016678348549E-3</v>
-      </c>
-      <c r="AI2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AG2" s="9">
         <f t="shared" si="0"/>
-        <v>2.3794810593877891E-3</v>
-      </c>
-      <c r="AJ2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AH2" s="9">
         <f t="shared" si="0"/>
-        <v>2.4166604509407233E-3</v>
-      </c>
-      <c r="AK2" s="4">
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AI2" s="9">
         <f t="shared" si="0"/>
-        <v>2.4538398424936575E-3</v>
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AJ2" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2269199212468287E-3</v>
+      </c>
+      <c r="AK2" s="9">
+        <f t="shared" si="0"/>
+        <v>1.2269199212468287E-3</v>
       </c>
     </row>
     <row r="3" spans="1:37">
@@ -45901,135 +45868,135 @@
       </c>
       <c r="E6" s="4">
         <f>E4*(1-'Calculations Etc'!$B$8)+E2*'Calculations Etc'!$B$8</f>
-        <v>8.6864578446400832E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="F6" s="4">
         <f>F4*(1-'Calculations Etc'!$B$8)+F2*'Calculations Etc'!$B$8</f>
-        <v>8.890944498181222E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="G6" s="4">
         <f>G4*(1-'Calculations Etc'!$B$8)+G2*'Calculations Etc'!$B$8</f>
-        <v>9.0954311517223597E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="H6" s="4">
         <f>H4*(1-'Calculations Etc'!$B$8)+H2*'Calculations Etc'!$B$8</f>
-        <v>9.2999178052634974E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="I6" s="4">
         <f>I4*(1-'Calculations Etc'!$B$8)+I2*'Calculations Etc'!$B$8</f>
-        <v>9.5044044588046361E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="J6" s="4">
         <f>J4*(1-'Calculations Etc'!$B$8)+J2*'Calculations Etc'!$B$8</f>
-        <v>9.7088911123457738E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="K6" s="4">
         <f>K4*(1-'Calculations Etc'!$B$8)+K2*'Calculations Etc'!$B$8</f>
-        <v>9.9133777658869126E-4</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="L6" s="4">
         <f>L4*(1-'Calculations Etc'!$B$8)+L2*'Calculations Etc'!$B$8</f>
-        <v>1.011786441942805E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="M6" s="4">
         <f>M4*(1-'Calculations Etc'!$B$8)+M2*'Calculations Etc'!$B$8</f>
-        <v>1.0322351072969188E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="N6" s="4">
         <f>N4*(1-'Calculations Etc'!$B$8)+N2*'Calculations Etc'!$B$8</f>
-        <v>1.0526837726510326E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="O6" s="4">
         <f>O4*(1-'Calculations Etc'!$B$8)+O2*'Calculations Etc'!$B$8</f>
-        <v>1.0731324380051463E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="P6" s="4">
         <f>P4*(1-'Calculations Etc'!$B$8)+P2*'Calculations Etc'!$B$8</f>
-        <v>1.0935811033592603E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="Q6" s="4">
         <f>Q4*(1-'Calculations Etc'!$B$8)+Q2*'Calculations Etc'!$B$8</f>
-        <v>1.1140297687133741E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="R6" s="4">
         <f>R4*(1-'Calculations Etc'!$B$8)+R2*'Calculations Etc'!$B$8</f>
-        <v>1.1344784340674879E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="S6" s="4">
         <f>S4*(1-'Calculations Etc'!$B$8)+S2*'Calculations Etc'!$B$8</f>
-        <v>1.1549270994216016E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="T6" s="4">
         <f>T4*(1-'Calculations Etc'!$B$8)+T2*'Calculations Etc'!$B$8</f>
-        <v>1.1753757647757154E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="U6" s="4">
         <f>U4*(1-'Calculations Etc'!$B$8)+U2*'Calculations Etc'!$B$8</f>
-        <v>1.1958244301298292E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="V6" s="4">
         <f>V4*(1-'Calculations Etc'!$B$8)+V2*'Calculations Etc'!$B$8</f>
-        <v>1.2162730954839432E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="W6" s="4">
         <f>W4*(1-'Calculations Etc'!$B$8)+W2*'Calculations Etc'!$B$8</f>
-        <v>1.2367217608380569E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="X6" s="4">
         <f>X4*(1-'Calculations Etc'!$B$8)+X2*'Calculations Etc'!$B$8</f>
-        <v>1.2571704261921707E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="Y6" s="4">
         <f>Y4*(1-'Calculations Etc'!$B$8)+Y2*'Calculations Etc'!$B$8</f>
-        <v>1.2776190915462845E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="Z6" s="4">
         <f>Z4*(1-'Calculations Etc'!$B$8)+Z2*'Calculations Etc'!$B$8</f>
-        <v>1.2980677569003982E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AA6" s="4">
         <f>AA4*(1-'Calculations Etc'!$B$8)+AA2*'Calculations Etc'!$B$8</f>
-        <v>1.3185164222545122E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AB6" s="4">
         <f>AB4*(1-'Calculations Etc'!$B$8)+AB2*'Calculations Etc'!$B$8</f>
-        <v>1.338965087608626E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AC6" s="4">
         <f>AC4*(1-'Calculations Etc'!$B$8)+AC2*'Calculations Etc'!$B$8</f>
-        <v>1.3594137529627398E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AD6" s="4">
         <f>AD4*(1-'Calculations Etc'!$B$8)+AD2*'Calculations Etc'!$B$8</f>
-        <v>1.3798624183168535E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AE6" s="4">
         <f>AE4*(1-'Calculations Etc'!$B$8)+AE2*'Calculations Etc'!$B$8</f>
-        <v>1.4003110836709673E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AF6" s="4">
         <f>AF4*(1-'Calculations Etc'!$B$8)+AF2*'Calculations Etc'!$B$8</f>
-        <v>1.4207597490250813E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AG6" s="4">
         <f>AG4*(1-'Calculations Etc'!$B$8)+AG2*'Calculations Etc'!$B$8</f>
-        <v>1.441208414379195E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AH6" s="4">
         <f>AH4*(1-'Calculations Etc'!$B$8)+AH2*'Calculations Etc'!$B$8</f>
-        <v>1.4616570797333088E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AI6" s="4">
         <f>AI4*(1-'Calculations Etc'!$B$8)+AI2*'Calculations Etc'!$B$8</f>
-        <v>1.4821057450874226E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AJ6" s="4">
         <f>AJ4*(1-'Calculations Etc'!$B$8)+AJ2*'Calculations Etc'!$B$8</f>
-        <v>1.5025544104415364E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
       <c r="AK6" s="4">
         <f>AK4*(1-'Calculations Etc'!$B$8)+AK2*'Calculations Etc'!$B$8</f>
-        <v>1.5230030757956503E-3</v>
+        <v>8.4819711910989455E-4</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -46356,7 +46323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -47533,7 +47500,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -48710,7 +48677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -49887,7 +49854,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -50010,7 +49977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -51042,7 +51009,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -52074,7 +52041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -53037,7 +53004,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -54069,7 +54036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -55032,7 +54999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -56068,7 +56035,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -57255,7 +57222,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -58179,7 +58146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58303,7 +58270,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58438,7 +58405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58600,7 +58567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58762,7 +58729,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -58891,7 +58858,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804A9106-3BA0-4B90-9845-AFCEFC0D7629}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>